<commit_message>
Fixed health uploader bugs.
</commit_message>
<xml_diff>
--- a/dashboard_loader/health_diabetes_uploader/health_diabetes.xlsx
+++ b/dashboard_loader/health_diabetes_uploader/health_diabetes.xlsx
@@ -110,7 +110,7 @@
     <numFmt numFmtId="165" formatCode="########\ ###\ ##0.0;\-########\ ###\ ##0.0;\–"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -131,12 +131,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -212,7 +206,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -240,77 +234,61 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -319,18 +297,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Microsoft Excel found an error in the formula you entered. Do you want to accept the correction proposed below?&#10;&#10;|&#10;&#10;• To accept the correction, click Yes.&#10;• To close this message and correct the formula yourself, click No. 16 2" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal_AIHW RoGS indicator concordance_NHA PI 13 4 yo health check" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 152" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal_2009 Attachment 7A.4_Tobacco" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal_ABS NHA PEx 2010 final version ACTIVE" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -358,6 +332,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -549,8 +527,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="94.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>